<commit_message>
major revision to structure
</commit_message>
<xml_diff>
--- a/docs/static/pilot-data-item-review.xlsx
+++ b/docs/static/pilot-data-item-review.xlsx
@@ -5,16 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\noahp\Box\Research\pools-projects\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\noahp\Box\Research\pools-projects\item-review-2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9C18A44D-8D78-4A79-BBFE-7F7C8451AB4C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{129ED03B-EDA1-4C06-9780-99DD2856D6DD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="11364" yWindow="60" windowWidth="11436" windowHeight="12096" xr2:uid="{A8F8FB6A-1449-4F11-B172-2E91181BEFB7}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{A8F8FB6A-1449-4F11-B172-2E91181BEFB7}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="EFA Results" sheetId="1" r:id="rId1"/>
+    <sheet name="CFA Results" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="206" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="138">
   <si>
     <t>permits students to acquire content knowledge. (1)</t>
   </si>
@@ -407,13 +409,55 @@
   </si>
   <si>
     <t>"skills such as…"</t>
+  </si>
+  <si>
+    <t>Enaging</t>
+  </si>
+  <si>
+    <t>Eff. Learn</t>
+  </si>
+  <si>
+    <t>Stud. Center</t>
+  </si>
+  <si>
+    <t>EL =~</t>
+  </si>
+  <si>
+    <t>SC =~</t>
+  </si>
+  <si>
+    <t>IN =~</t>
+  </si>
+  <si>
+    <t>EN =~</t>
+  </si>
+  <si>
+    <t>Effective learning is defined as learning in which students masterfully acquire and utilize relevant</t>
+  </si>
+  <si>
+    <t>new knowledge and/or skills, as witnessed through application and assessment that occur within or outside</t>
+  </si>
+  <si>
+    <t>the immediate classroom.</t>
+  </si>
+  <si>
+    <t>promotes higher-order thinking skills such as analysis, synthesis, and evaluation. (11)</t>
+  </si>
+  <si>
+    <t>is effective for building content knowledge. (4new)</t>
+  </si>
+  <si>
+    <t>is effective for building conceptual understanding. (18new)</t>
+  </si>
+  <si>
+    <t>permits student interaction with the teacher. (5new)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -460,6 +504,20 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="3">
@@ -508,7 +566,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -531,6 +589,18 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -849,8 +919,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D5FA4E3-2DA5-47E8-8CAF-2521EC0A58C9}">
   <dimension ref="A1:G43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A46" sqref="A46"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15:XFD15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1715,6 +1785,419 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DD28136F-7D6E-4B98-A46B-9C4F36E79E1B}">
+  <dimension ref="A1:G42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="145" zoomScaleNormal="145" workbookViewId="0">
+      <selection activeCell="A43" sqref="A43"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="82.44140625" customWidth="1"/>
+    <col min="2" max="2" width="6.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.77734375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="7.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A1" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="C1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D1" t="s">
+        <v>126</v>
+      </c>
+      <c r="E1" t="s">
+        <v>116</v>
+      </c>
+      <c r="F1" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="10"/>
+      <c r="G2" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" s="11"/>
+      <c r="G3" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" s="11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4">
+        <v>0.85</v>
+      </c>
+      <c r="G4" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" s="11"/>
+      <c r="B5" t="s">
+        <v>60</v>
+      </c>
+      <c r="C5">
+        <v>0.85299999999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" s="11" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
+        <v>61</v>
+      </c>
+      <c r="C6">
+        <v>0.80200000000000005</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" s="11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>65</v>
+      </c>
+      <c r="C7">
+        <v>0.752</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" s="11"/>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" s="11" t="s">
+        <v>134</v>
+      </c>
+      <c r="B9" t="s">
+        <v>67</v>
+      </c>
+      <c r="C9">
+        <v>0.83199999999999996</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="B10" t="s">
+        <v>71</v>
+      </c>
+      <c r="C10">
+        <v>0.78500000000000003</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" s="11"/>
+      <c r="B11" t="s">
+        <v>74</v>
+      </c>
+      <c r="C11">
+        <v>0.85499999999999998</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" s="11" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" s="11" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" s="8" t="s">
+        <v>117</v>
+      </c>
+      <c r="B14" s="8"/>
+      <c r="C14" s="8"/>
+      <c r="D14" s="8"/>
+      <c r="E14" s="8"/>
+      <c r="F14" s="8"/>
+    </row>
+    <row r="15" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A15" s="10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" t="s">
+        <v>76</v>
+      </c>
+      <c r="D15">
+        <v>0.77800000000000002</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" s="11"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A17" s="11" t="s">
+        <v>21</v>
+      </c>
+      <c r="B17" t="s">
+        <v>78</v>
+      </c>
+      <c r="D17">
+        <v>0.72099999999999997</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A18" s="11" t="s">
+        <v>22</v>
+      </c>
+      <c r="B18" t="s">
+        <v>79</v>
+      </c>
+      <c r="D18">
+        <v>0.82199999999999995</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="11" t="s">
+        <v>23</v>
+      </c>
+      <c r="B19" t="s">
+        <v>80</v>
+      </c>
+      <c r="D19">
+        <v>0.84399999999999997</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="B20" t="s">
+        <v>81</v>
+      </c>
+      <c r="D20">
+        <v>0.80400000000000005</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A21" s="11"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="11" t="s">
+        <v>30</v>
+      </c>
+      <c r="B22" t="s">
+        <v>87</v>
+      </c>
+      <c r="D22">
+        <v>0.79200000000000004</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="17.399999999999999" x14ac:dyDescent="0.3">
+      <c r="A23" s="12" t="s">
+        <v>116</v>
+      </c>
+      <c r="B23" s="12"/>
+      <c r="C23" s="12"/>
+      <c r="D23" s="12"/>
+      <c r="E23" s="12"/>
+      <c r="F23" s="12"/>
+    </row>
+    <row r="24" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="10"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="B25" t="s">
+        <v>89</v>
+      </c>
+      <c r="E25">
+        <v>0.84</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="11"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="11"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="B28" t="s">
+        <v>92</v>
+      </c>
+      <c r="E28">
+        <v>0.55300000000000005</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" s="11" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="B30" t="s">
+        <v>93</v>
+      </c>
+      <c r="E30">
+        <v>0.85199999999999998</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B31" t="s">
+        <v>94</v>
+      </c>
+      <c r="E31">
+        <v>0.90200000000000002</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A32" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B32" t="s">
+        <v>95</v>
+      </c>
+      <c r="E32">
+        <v>0.84799999999999998</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="B33" t="s">
+        <v>98</v>
+      </c>
+      <c r="E33">
+        <v>0.85399999999999998</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A34" s="13" t="s">
+        <v>115</v>
+      </c>
+      <c r="B34" s="13"/>
+      <c r="C34" s="13"/>
+      <c r="D34" s="13"/>
+      <c r="E34" s="13"/>
+      <c r="F34" s="13"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="B35" t="s">
+        <v>100</v>
+      </c>
+      <c r="F35">
+        <v>0.82599999999999996</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" s="11" t="s">
+        <v>45</v>
+      </c>
+      <c r="B36" t="s">
+        <v>102</v>
+      </c>
+      <c r="F36">
+        <v>0.69899999999999995</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" s="11" t="s">
+        <v>46</v>
+      </c>
+      <c r="B37" t="s">
+        <v>103</v>
+      </c>
+      <c r="F37">
+        <v>0.78800000000000003</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" s="11" t="s">
+        <v>48</v>
+      </c>
+      <c r="B38" t="s">
+        <v>105</v>
+      </c>
+      <c r="F38">
+        <v>0.69799999999999995</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A39" s="11" t="s">
+        <v>49</v>
+      </c>
+      <c r="B39" t="s">
+        <v>106</v>
+      </c>
+      <c r="F39">
+        <v>0.79800000000000004</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A40" s="11"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A41" s="11"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A42" s="11" t="s">
+        <v>55</v>
+      </c>
+      <c r="B42" t="s">
+        <v>112</v>
+      </c>
+      <c r="F42">
+        <v>0.67100000000000004</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="3">
+    <mergeCell ref="A14:F14"/>
+    <mergeCell ref="A23:F23"/>
+    <mergeCell ref="A34:F34"/>
+  </mergeCells>
+  <conditionalFormatting sqref="C35:E42 D2:F13 C24:D33 F24:F33 C15:C22 E15:F22">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="num" val="0"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color theme="0"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19ABCA08-7523-4AB0-9470-3224D9489E24}">
   <dimension ref="A1:F61"/>
   <sheetViews>
@@ -2922,4 +3405,877 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C0F31054-5E4F-4DDB-B92F-27F999673E60}">
+  <dimension ref="A1:G42"/>
+  <sheetViews>
+    <sheetView topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2:G42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>57</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>0.81799999999999995</v>
+      </c>
+      <c r="G2">
+        <v>0.81799999999999995</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3">
+        <v>0.96099999999999997</v>
+      </c>
+      <c r="C3">
+        <v>0.03</v>
+      </c>
+      <c r="D3">
+        <v>32.295000000000002</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0.78600000000000003</v>
+      </c>
+      <c r="G3">
+        <v>0.78600000000000003</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B4">
+        <v>1.04</v>
+      </c>
+      <c r="C4">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="D4">
+        <v>36.427999999999997</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4">
+        <v>0.85</v>
+      </c>
+      <c r="G4">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B5">
+        <v>1.0429999999999999</v>
+      </c>
+      <c r="C5">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="D5">
+        <v>37.591000000000001</v>
+      </c>
+      <c r="E5">
+        <v>0</v>
+      </c>
+      <c r="F5">
+        <v>0.85299999999999998</v>
+      </c>
+      <c r="G5">
+        <v>0.85299999999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>61</v>
+      </c>
+      <c r="B6">
+        <v>0.98099999999999998</v>
+      </c>
+      <c r="C6">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="D6">
+        <v>29.62</v>
+      </c>
+      <c r="E6">
+        <v>0</v>
+      </c>
+      <c r="F6">
+        <v>0.80200000000000005</v>
+      </c>
+      <c r="G6">
+        <v>0.80200000000000005</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7">
+        <v>0.95399999999999996</v>
+      </c>
+      <c r="C7">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="D7">
+        <v>27.564</v>
+      </c>
+      <c r="E7">
+        <v>0</v>
+      </c>
+      <c r="F7">
+        <v>0.78</v>
+      </c>
+      <c r="G7">
+        <v>0.78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>65</v>
+      </c>
+      <c r="B8">
+        <v>0.92</v>
+      </c>
+      <c r="C8">
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="D8">
+        <v>25.167000000000002</v>
+      </c>
+      <c r="E8">
+        <v>0</v>
+      </c>
+      <c r="F8">
+        <v>0.752</v>
+      </c>
+      <c r="G8">
+        <v>0.752</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>66</v>
+      </c>
+      <c r="B9">
+        <v>1.0089999999999999</v>
+      </c>
+      <c r="C9">
+        <v>3.1E-2</v>
+      </c>
+      <c r="D9">
+        <v>32.551000000000002</v>
+      </c>
+      <c r="E9">
+        <v>0</v>
+      </c>
+      <c r="F9">
+        <v>0.82499999999999996</v>
+      </c>
+      <c r="G9">
+        <v>0.82499999999999996</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>67</v>
+      </c>
+      <c r="B10">
+        <v>1.0169999999999999</v>
+      </c>
+      <c r="C10">
+        <v>3.3000000000000002E-2</v>
+      </c>
+      <c r="D10">
+        <v>31.152000000000001</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
+        <v>0.83199999999999996</v>
+      </c>
+      <c r="G10">
+        <v>0.83199999999999996</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>71</v>
+      </c>
+      <c r="B11">
+        <v>0.96</v>
+      </c>
+      <c r="C11">
+        <v>0.03</v>
+      </c>
+      <c r="D11">
+        <v>31.834</v>
+      </c>
+      <c r="E11">
+        <v>0</v>
+      </c>
+      <c r="F11">
+        <v>0.78500000000000003</v>
+      </c>
+      <c r="G11">
+        <v>0.78500000000000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>72</v>
+      </c>
+      <c r="B12">
+        <v>0.91400000000000003</v>
+      </c>
+      <c r="C12">
+        <v>3.1E-2</v>
+      </c>
+      <c r="D12">
+        <v>29.027000000000001</v>
+      </c>
+      <c r="E12">
+        <v>0</v>
+      </c>
+      <c r="F12">
+        <v>0.747</v>
+      </c>
+      <c r="G12">
+        <v>0.747</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>73</v>
+      </c>
+      <c r="B13">
+        <v>0.81299999999999994</v>
+      </c>
+      <c r="C13">
+        <v>3.9E-2</v>
+      </c>
+      <c r="D13">
+        <v>20.917999999999999</v>
+      </c>
+      <c r="E13">
+        <v>0</v>
+      </c>
+      <c r="F13">
+        <v>0.66500000000000004</v>
+      </c>
+      <c r="G13">
+        <v>0.66500000000000004</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>74</v>
+      </c>
+      <c r="B14">
+        <v>1.046</v>
+      </c>
+      <c r="C14">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="D14">
+        <v>36.037999999999997</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
+        <v>0.85499999999999998</v>
+      </c>
+      <c r="G14">
+        <v>0.85499999999999998</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>76</v>
+      </c>
+      <c r="B16">
+        <v>1</v>
+      </c>
+      <c r="F16">
+        <v>0.77800000000000002</v>
+      </c>
+      <c r="G16">
+        <v>0.77800000000000002</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>77</v>
+      </c>
+      <c r="B17">
+        <v>0.86599999999999999</v>
+      </c>
+      <c r="C17">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="D17">
+        <v>18.736000000000001</v>
+      </c>
+      <c r="E17">
+        <v>0</v>
+      </c>
+      <c r="F17">
+        <v>0.67400000000000004</v>
+      </c>
+      <c r="G17">
+        <v>0.67400000000000004</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>78</v>
+      </c>
+      <c r="B18">
+        <v>0.92700000000000005</v>
+      </c>
+      <c r="C18">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="D18">
+        <v>17.786000000000001</v>
+      </c>
+      <c r="E18">
+        <v>0</v>
+      </c>
+      <c r="F18">
+        <v>0.72099999999999997</v>
+      </c>
+      <c r="G18">
+        <v>0.72099999999999997</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>79</v>
+      </c>
+      <c r="B19">
+        <v>1.0569999999999999</v>
+      </c>
+      <c r="C19">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="D19">
+        <v>22.832999999999998</v>
+      </c>
+      <c r="E19">
+        <v>0</v>
+      </c>
+      <c r="F19">
+        <v>0.82199999999999995</v>
+      </c>
+      <c r="G19">
+        <v>0.82199999999999995</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>80</v>
+      </c>
+      <c r="B20">
+        <v>1.085</v>
+      </c>
+      <c r="C20">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="D20">
+        <v>24.149000000000001</v>
+      </c>
+      <c r="E20">
+        <v>0</v>
+      </c>
+      <c r="F20">
+        <v>0.84399999999999997</v>
+      </c>
+      <c r="G20">
+        <v>0.84399999999999997</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>81</v>
+      </c>
+      <c r="B21">
+        <v>1.0329999999999999</v>
+      </c>
+      <c r="C21">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="D21">
+        <v>21.190999999999999</v>
+      </c>
+      <c r="E21">
+        <v>0</v>
+      </c>
+      <c r="F21">
+        <v>0.80400000000000005</v>
+      </c>
+      <c r="G21">
+        <v>0.80400000000000005</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>83</v>
+      </c>
+      <c r="B22">
+        <v>1.0049999999999999</v>
+      </c>
+      <c r="C22">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="D22">
+        <v>19.593</v>
+      </c>
+      <c r="E22">
+        <v>0</v>
+      </c>
+      <c r="F22">
+        <v>0.78200000000000003</v>
+      </c>
+      <c r="G22">
+        <v>0.78200000000000003</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>87</v>
+      </c>
+      <c r="B23">
+        <v>1.018</v>
+      </c>
+      <c r="C23">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="D23">
+        <v>19.821999999999999</v>
+      </c>
+      <c r="E23">
+        <v>0</v>
+      </c>
+      <c r="F23">
+        <v>0.79200000000000004</v>
+      </c>
+      <c r="G23">
+        <v>0.79200000000000004</v>
+      </c>
+    </row>
+    <row r="24" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="25" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>88</v>
+      </c>
+      <c r="B25">
+        <v>1</v>
+      </c>
+      <c r="F25">
+        <v>0.75700000000000001</v>
+      </c>
+      <c r="G25">
+        <v>0.75700000000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>89</v>
+      </c>
+      <c r="B26">
+        <v>1.1100000000000001</v>
+      </c>
+      <c r="C26">
+        <v>4.4999999999999998E-2</v>
+      </c>
+      <c r="D26">
+        <v>24.613</v>
+      </c>
+      <c r="E26">
+        <v>0</v>
+      </c>
+      <c r="F26">
+        <v>0.84</v>
+      </c>
+      <c r="G26">
+        <v>0.84</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>90</v>
+      </c>
+      <c r="B27">
+        <v>1.06</v>
+      </c>
+      <c r="C27">
+        <v>4.9000000000000002E-2</v>
+      </c>
+      <c r="D27">
+        <v>21.672999999999998</v>
+      </c>
+      <c r="E27">
+        <v>0</v>
+      </c>
+      <c r="F27">
+        <v>0.80300000000000005</v>
+      </c>
+      <c r="G27">
+        <v>0.80300000000000005</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>91</v>
+      </c>
+      <c r="B28">
+        <v>1.0660000000000001</v>
+      </c>
+      <c r="C28">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="D28">
+        <v>23.026</v>
+      </c>
+      <c r="E28">
+        <v>0</v>
+      </c>
+      <c r="F28">
+        <v>0.80600000000000005</v>
+      </c>
+      <c r="G28">
+        <v>0.80600000000000005</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>92</v>
+      </c>
+      <c r="B29">
+        <v>0.73099999999999998</v>
+      </c>
+      <c r="C29">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="D29">
+        <v>12.943</v>
+      </c>
+      <c r="E29">
+        <v>0</v>
+      </c>
+      <c r="F29">
+        <v>0.55300000000000005</v>
+      </c>
+      <c r="G29">
+        <v>0.55300000000000005</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>93</v>
+      </c>
+      <c r="B30">
+        <v>1.1259999999999999</v>
+      </c>
+      <c r="C30">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="D30">
+        <v>21.716999999999999</v>
+      </c>
+      <c r="E30">
+        <v>0</v>
+      </c>
+      <c r="F30">
+        <v>0.85199999999999998</v>
+      </c>
+      <c r="G30">
+        <v>0.85199999999999998</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>94</v>
+      </c>
+      <c r="B31">
+        <v>1.1919999999999999</v>
+      </c>
+      <c r="C31">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="D31">
+        <v>20.542999999999999</v>
+      </c>
+      <c r="E31">
+        <v>0</v>
+      </c>
+      <c r="F31">
+        <v>0.90200000000000002</v>
+      </c>
+      <c r="G31">
+        <v>0.90200000000000002</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>95</v>
+      </c>
+      <c r="B32">
+        <v>1.121</v>
+      </c>
+      <c r="C32">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="D32">
+        <v>21.584</v>
+      </c>
+      <c r="E32">
+        <v>0</v>
+      </c>
+      <c r="F32">
+        <v>0.84799999999999998</v>
+      </c>
+      <c r="G32">
+        <v>0.84799999999999998</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>98</v>
+      </c>
+      <c r="B33">
+        <v>1.129</v>
+      </c>
+      <c r="C33">
+        <v>6.2E-2</v>
+      </c>
+      <c r="D33">
+        <v>18.324000000000002</v>
+      </c>
+      <c r="E33">
+        <v>0</v>
+      </c>
+      <c r="F33">
+        <v>0.85399999999999998</v>
+      </c>
+      <c r="G33">
+        <v>0.85399999999999998</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="35" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>100</v>
+      </c>
+      <c r="B35">
+        <v>1</v>
+      </c>
+      <c r="F35">
+        <v>0.82599999999999996</v>
+      </c>
+      <c r="G35">
+        <v>0.82599999999999996</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>102</v>
+      </c>
+      <c r="B36">
+        <v>0.84599999999999997</v>
+      </c>
+      <c r="C36">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="D36">
+        <v>22.146000000000001</v>
+      </c>
+      <c r="E36">
+        <v>0</v>
+      </c>
+      <c r="F36">
+        <v>0.69899999999999995</v>
+      </c>
+      <c r="G36">
+        <v>0.69899999999999995</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>103</v>
+      </c>
+      <c r="B37">
+        <v>0.95399999999999996</v>
+      </c>
+      <c r="C37">
+        <v>3.7999999999999999E-2</v>
+      </c>
+      <c r="D37">
+        <v>24.957000000000001</v>
+      </c>
+      <c r="E37">
+        <v>0</v>
+      </c>
+      <c r="F37">
+        <v>0.78800000000000003</v>
+      </c>
+      <c r="G37">
+        <v>0.78800000000000003</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>105</v>
+      </c>
+      <c r="B38">
+        <v>0.84499999999999997</v>
+      </c>
+      <c r="C38">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="D38">
+        <v>19.242000000000001</v>
+      </c>
+      <c r="E38">
+        <v>0</v>
+      </c>
+      <c r="F38">
+        <v>0.69799999999999995</v>
+      </c>
+      <c r="G38">
+        <v>0.69799999999999995</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>106</v>
+      </c>
+      <c r="B39">
+        <v>0.96599999999999997</v>
+      </c>
+      <c r="C39">
+        <v>0.04</v>
+      </c>
+      <c r="D39">
+        <v>24.27</v>
+      </c>
+      <c r="E39">
+        <v>0</v>
+      </c>
+      <c r="F39">
+        <v>0.79800000000000004</v>
+      </c>
+      <c r="G39">
+        <v>0.79800000000000004</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>110</v>
+      </c>
+      <c r="B40">
+        <v>0.84899999999999998</v>
+      </c>
+      <c r="C40">
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="D40">
+        <v>19.253</v>
+      </c>
+      <c r="E40">
+        <v>0</v>
+      </c>
+      <c r="F40">
+        <v>0.70099999999999996</v>
+      </c>
+      <c r="G40">
+        <v>0.70099999999999996</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>111</v>
+      </c>
+      <c r="B41">
+        <v>0.48899999999999999</v>
+      </c>
+      <c r="C41">
+        <v>5.5E-2</v>
+      </c>
+      <c r="D41">
+        <v>8.9510000000000005</v>
+      </c>
+      <c r="E41">
+        <v>0</v>
+      </c>
+      <c r="F41">
+        <v>0.40400000000000003</v>
+      </c>
+      <c r="G41">
+        <v>0.40400000000000003</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>112</v>
+      </c>
+      <c r="B42">
+        <v>0.81200000000000006</v>
+      </c>
+      <c r="C42">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="D42">
+        <v>17.715</v>
+      </c>
+      <c r="E42">
+        <v>0</v>
+      </c>
+      <c r="F42">
+        <v>0.67100000000000004</v>
+      </c>
+      <c r="G42">
+        <v>0.67100000000000004</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>